<commit_message>
rerunning ch 6 PN output
</commit_message>
<xml_diff>
--- a/Ch_6_Form/6 Graphs.xlsx
+++ b/Ch_6_Form/6 Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Github\PhD\Ch_6_Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63BCB95-118F-49B3-A477-8C174711C59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A87EF4E-C729-447C-9A8E-8F9738FD12D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{1ABE4724-14B1-4801-819D-892587CA02C5}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{1ABE4724-14B1-4801-819D-892587CA02C5}"/>
   </bookViews>
   <sheets>
     <sheet name="nuc foot" sheetId="1" r:id="rId1"/>
@@ -24483,7 +24483,7 @@
                     <c:v>39.603253615283961</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>32.523008490727989</c:v>
+                    <c:v>32.523102356104999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -24498,7 +24498,7 @@
                     <c:v>39.603253615283961</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>32.523008490727989</c:v>
+                    <c:v>32.523102356104999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -24695,7 +24695,7 @@
                     <c:v>38.994705327151109</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>34.32899009903602</c:v>
+                    <c:v>34.329239056907994</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -24710,7 +24710,7 @@
                     <c:v>38.994705327151109</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>34.32899009903602</c:v>
+                    <c:v>34.329239056907994</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -24817,7 +24817,7 @@
                     <c:v>39.120556731791503</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>43.893535616929</c:v>
+                    <c:v>43.894060309150973</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -24832,7 +24832,7 @@
                     <c:v>39.120556731791503</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>43.893535616929</c:v>
+                    <c:v>43.894060309150973</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -24988,7 +24988,7 @@
                     <c:v>39.612457096101295</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>39.996234637442996</c:v>
+                    <c:v>39.998646913039011</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -25003,7 +25003,7 @@
                     <c:v>39.612457096101295</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>39.996234637442996</c:v>
+                    <c:v>39.998646913039011</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -25557,16 +25557,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>32.523008490727989</c:v>
+                    <c:v>32.523102356104999</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>34.32899009903602</c:v>
+                    <c:v>34.329239056907994</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.893535616929</c:v>
+                    <c:v>43.894060309150973</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>39.996234637442996</c:v>
+                    <c:v>39.998646913039011</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -25578,16 +25578,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>32.523008490727989</c:v>
+                    <c:v>32.523102356104999</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>34.32899009903602</c:v>
+                    <c:v>34.329239056907994</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.893535616929</c:v>
+                    <c:v>43.894060309150973</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>39.996234637442996</c:v>
+                    <c:v>39.998646913039011</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -25707,16 +25707,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>32.523008490727989</c:v>
+                    <c:v>32.523102356104999</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>34.32899009903602</c:v>
+                    <c:v>34.329239056907994</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.893535616929</c:v>
+                    <c:v>43.894060309150973</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>39.996234637442996</c:v>
+                    <c:v>39.998646913039011</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -25728,16 +25728,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>32.523008490727989</c:v>
+                    <c:v>32.523102356104999</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>34.32899009903602</c:v>
+                    <c:v>34.329239056907994</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>43.893535616929</c:v>
+                    <c:v>43.894060309150973</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>39.996234637442996</c:v>
+                    <c:v>39.998646913039011</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -26815,7 +26815,7 @@
                     <c:v>39.603253615283961</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>32.523008490727989</c:v>
+                    <c:v>32.523102356104999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -26830,7 +26830,7 @@
                     <c:v>39.603253615283961</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>32.523008490727989</c:v>
+                    <c:v>32.523102356104999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -27027,7 +27027,7 @@
                     <c:v>38.994705327151109</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>34.32899009903602</c:v>
+                    <c:v>34.329239056907994</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -27042,7 +27042,7 @@
                     <c:v>38.994705327151109</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>34.32899009903602</c:v>
+                    <c:v>34.329239056907994</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -27149,7 +27149,7 @@
                     <c:v>39.120556731791503</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>43.893535616929</c:v>
+                    <c:v>43.894060309150973</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -27164,7 +27164,7 @@
                     <c:v>39.120556731791503</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>43.893535616929</c:v>
+                    <c:v>43.894060309150973</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -27320,7 +27320,7 @@
                     <c:v>39.612457096101295</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>39.996234637442996</c:v>
+                    <c:v>39.998646913039011</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -27335,7 +27335,7 @@
                     <c:v>39.612457096101295</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>39.996234637442996</c:v>
+                    <c:v>39.998646913039011</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -27863,7 +27863,7 @@
                     <c:v>39.603253615283961</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>32.523050319513999</c:v>
+                    <c:v>32.523161582785008</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -27878,7 +27878,7 @@
                     <c:v>39.603253615283961</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>32.523050319513999</c:v>
+                    <c:v>32.523161582785008</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -28075,7 +28075,7 @@
                     <c:v>96.232645765229094</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>55.871600420300609</c:v>
+                    <c:v>55.87153053789001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -28090,7 +28090,7 @@
                     <c:v>96.232645765229094</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>55.871600420300609</c:v>
+                    <c:v>55.87153053789001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -28197,7 +28197,7 @@
                     <c:v>96.168894014132306</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>56.526610306574014</c:v>
+                    <c:v>56.526462709865996</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -28212,7 +28212,7 @@
                     <c:v>96.168894014132306</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>56.526610306574014</c:v>
+                    <c:v>56.526462709865996</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -28368,7 +28368,7 @@
                     <c:v>96.1658297226451</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>56.526598636073004</c:v>
+                    <c:v>56.526609547513999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -28383,7 +28383,7 @@
                     <c:v>96.1658297226451</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>56.526598636073004</c:v>
+                    <c:v>56.526609547513999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -28919,16 +28919,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>32.523050319513999</c:v>
+                    <c:v>32.523161582785008</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>55.871600420300609</c:v>
+                    <c:v>55.87153053789001</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>56.526610306574014</c:v>
+                    <c:v>56.526462709865996</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>56.526598636073004</c:v>
+                    <c:v>56.526609547513999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -28940,16 +28940,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>32.523050319513999</c:v>
+                    <c:v>32.523161582785008</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>55.871600420300609</c:v>
+                    <c:v>55.87153053789001</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>56.526610306574014</c:v>
+                    <c:v>56.526462709865996</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>56.526598636073004</c:v>
+                    <c:v>56.526609547513999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -29069,16 +29069,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>32.523050319513999</c:v>
+                    <c:v>32.523161582785008</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>55.871600420300609</c:v>
+                    <c:v>55.87153053789001</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>56.526610306574014</c:v>
+                    <c:v>56.526462709865996</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>56.526598636073004</c:v>
+                    <c:v>56.526609547513999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -29090,16 +29090,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>32.523050319513999</c:v>
+                    <c:v>32.523161582785008</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>55.871600420300609</c:v>
+                    <c:v>55.87153053789001</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>56.526610306574014</c:v>
+                    <c:v>56.526462709865996</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>56.526598636073004</c:v>
+                    <c:v>56.526609547513999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -31218,7 +31218,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>syls3</c:v>
+                  <c:v>foot_syls4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -31249,10 +31249,29 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.7309700897940994E-2"/>
-                  <c:y val="-2.9619747414658181E-2"/>
+                  <c:x val="3.3044084704736007E-2"/>
+                  <c:y val="-3.3125832889491912E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -31261,7 +31280,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.12394822006472492"/>
+                      <c:h val="7.0603492398287129E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-4F58-43DB-A30E-F6CB6FA46978}"/>
                 </c:ext>
@@ -31335,7 +31361,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.958634009794029</c:v>
+                  <c:v>17.637018199837321</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31356,7 +31382,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>syls2</c:v>
+                  <c:v>foot_syls3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -31387,8 +31413,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.3634244834345219E-2"/>
-                  <c:y val="7.3755362742058406E-3"/>
+                  <c:x val="4.2384835560081852E-2"/>
+                  <c:y val="-5.4337911920860245E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -31421,8 +31447,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.10653526936775758"/>
-                      <c:h val="6.6447487494346438E-2"/>
+                      <c:w val="0.12502793946873145"/>
+                      <c:h val="7.5700200903061995E-2"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -31520,7 +31546,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>syls1</c:v>
+                  <c:v>foot_syls2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -31550,8 +31576,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.7659757435577937E-2"/>
-                  <c:y val="4.9220361106923289E-3"/>
+                  <c:x val="9.7046809778272396E-3"/>
+                  <c:y val="-9.9096907859985914E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -31635,7 +31661,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.332887019907195</c:v>
+                  <c:v>16.945460824541019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31656,7 +31682,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>syls0</c:v>
+                  <c:v>foot_syls1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -31687,8 +31713,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.8211730200932777E-2"/>
-                  <c:y val="-3.9350652430039032E-2"/>
+                  <c:x val="5.1621580175786885E-2"/>
+                  <c:y val="-6.2044635184329136E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -31773,7 +31799,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.439969192802881</c:v>
+                  <c:v>19.491919596031121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31908,28 +31934,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-IE" sz="900" b="0" i="1">
+                  <a:rPr lang="en-IE" sz="900" b="0" i="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>f</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-IE" sz="900" b="0" baseline="-25000">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>0</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-IE" sz="900" b="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> (ST)</a:t>
+                  <a:t>slope (ST/sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -31978,9 +31988,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18314614379236571"/>
-          <c:y val="0.12853740535401165"/>
-          <c:w val="0.23318072738624382"/>
+          <c:x val="0.18781779477873961"/>
+          <c:y val="0.14269701756015982"/>
+          <c:w val="0.39058580276308075"/>
           <c:h val="0.28341185185185186"/>
         </c:manualLayout>
       </c:layout>
@@ -32089,7 +32099,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>syls3</c:v>
+                  <c:v>foot_syls4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -32130,7 +32140,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.77</c:v>
+                  <c:v>2.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -32151,7 +32161,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>syls2</c:v>
+                  <c:v>foot_syls3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -32213,7 +32223,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>syls1</c:v>
+                  <c:v>foot_syls2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -32254,7 +32264,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.73</c:v>
+                  <c:v>2.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -32275,7 +32285,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>syls0</c:v>
+                  <c:v>foot_syls1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -32316,7 +32326,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.67</c:v>
+                  <c:v>2.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -32451,28 +32461,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-IE" sz="900" b="0" i="1">
+                  <a:rPr lang="en-IE" sz="900" b="0" i="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>f</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-IE" sz="900" b="0" baseline="-25000">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>0</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-IE" sz="900" b="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> (ST)</a:t>
+                  <a:t>slope (log[ST/sec])</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -32523,7 +32517,7 @@
           <c:yMode val="edge"/>
           <c:x val="9.0809748534842333E-2"/>
           <c:y val="0.13839592592592589"/>
-          <c:w val="0.28227747892844907"/>
+          <c:w val="0.38907865178399059"/>
           <c:h val="0.32104148148148148"/>
         </c:manualLayout>
       </c:layout>
@@ -32758,16 +32752,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.0306245130913101</c:v>
+                    <c:v>0.91045775647741989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1528372421283346</c:v>
+                    <c:v>0.87820526092814033</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.14725350680003</c:v>
+                    <c:v>0.86641593967474018</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.1431796435623323</c:v>
+                    <c:v>0.89705323721548025</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -32779,16 +32773,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.0306245130913101</c:v>
+                    <c:v>0.91045775647741989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1528372421283346</c:v>
+                    <c:v>0.87820526092814033</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.14725350680003</c:v>
+                    <c:v>0.86641593967474018</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.1431796435623323</c:v>
+                    <c:v>0.89705323721548025</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -32800,16 +32794,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>syls0</c:v>
+                  <c:v>foot_syls1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>syls1</c:v>
+                  <c:v>foot_syls2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>syls2</c:v>
+                  <c:v>foot_syls3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>syls3</c:v>
+                  <c:v>foot_syls4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -32821,16 +32815,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.25</c:v>
+                  <c:v>2.3199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.19</c:v>
+                  <c:v>2.91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.25</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.74</c:v>
+                  <c:v>2.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -33248,16 +33242,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>0.42554607282795009</c:v>
+                    <c:v>0.92989045444073026</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.93827991702499003</c:v>
+                    <c:v>0.86846361377577996</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.91107570000120996</c:v>
+                    <c:v>0.95696662049842995</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.91586236385601993</c:v>
+                    <c:v>0.32087840727744998</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -33269,16 +33263,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>0.42554607282795009</c:v>
+                    <c:v>0.92989045444073026</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.93827991702499003</c:v>
+                    <c:v>0.86846361377577996</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.91107570000120996</c:v>
+                    <c:v>0.95696662049842995</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.91586236385601993</c:v>
+                    <c:v>0.32087840727744998</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -33290,16 +33284,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>syls0</c:v>
+                  <c:v>foot_syls1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>syls1</c:v>
+                  <c:v>foot_syls2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>syls2</c:v>
+                  <c:v>foot_syls3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>syls3</c:v>
+                  <c:v>foot_syls4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -33311,16 +33305,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.67</c:v>
+                  <c:v>2.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.73</c:v>
+                  <c:v>2.83</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.77</c:v>
+                  <c:v>2.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -33714,16 +33708,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>syls0</c:v>
+                  <c:v>foot_syls1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>syls1</c:v>
+                  <c:v>foot_syls2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>syls2</c:v>
+                  <c:v>foot_syls3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>syls3</c:v>
+                  <c:v>foot_syls4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -33735,16 +33729,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.25</c:v>
+                  <c:v>2.3199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.19</c:v>
+                  <c:v>2.91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.25</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.74</c:v>
+                  <c:v>2.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34156,16 +34150,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>syls0</c:v>
+                  <c:v>foot_syls1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>syls1</c:v>
+                  <c:v>foot_syls2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>syls2</c:v>
+                  <c:v>foot_syls3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>syls3</c:v>
+                  <c:v>foot_syls4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -34177,16 +34171,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.67</c:v>
+                  <c:v>2.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.73</c:v>
+                  <c:v>2.83</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.77</c:v>
+                  <c:v>2.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34400,6 +34394,866 @@
 </file>
 
 <file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17260755106142528"/>
+          <c:y val="5.3600091302687433E-2"/>
+          <c:w val="0.63079731274731721"/>
+          <c:h val="0.783136730163979"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pn slope exc'!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>foot_syls4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="E7298A"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-E698-4A5F-BDE5-6E8233C84A0C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.3044084704736007E-2"/>
+                  <c:y val="-3.3125832889491912E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.12394822006472492"/>
+                      <c:h val="7.0603492398287129E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E698-4A5F-BDE5-6E8233C84A0C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:srgbClr val="E7298A"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDash"/>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pn slope exc'!$B$20:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pn slope exc'!$D$20:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.637018199837321</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E698-4A5F-BDE5-6E8233C84A0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pn slope exc'!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>foot_syls3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="47298A"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-E698-4A5F-BDE5-6E8233C84A0C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.2384835560081852E-2"/>
+                  <c:y val="-5.4337911920860245E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.12502793946873145"/>
+                      <c:h val="7.5700200903061995E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-E698-4A5F-BDE5-6E8233C84A0C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:srgbClr val="47298A"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pn slope exc'!$B$18:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pn slope exc'!$D$18:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.17414536944306</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E698-4A5F-BDE5-6E8233C84A0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pn slope exc'!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>foot_syls2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="D95F02"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-E698-4A5F-BDE5-6E8233C84A0C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.7046809778272396E-3"/>
+                  <c:y val="-9.9096907859985914E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-E698-4A5F-BDE5-6E8233C84A0C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:srgbClr val="D95F02"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pn slope exc'!$B$16:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pn slope exc'!$D$16:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.945460824541019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-E698-4A5F-BDE5-6E8233C84A0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pn slope exc'!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>foot_syls1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="1B9E77"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-E698-4A5F-BDE5-6E8233C84A0C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.1621580175786885E-2"/>
+                  <c:y val="-6.2044635184329136E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-E698-4A5F-BDE5-6E8233C84A0C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25400">
+                      <a:solidFill>
+                        <a:srgbClr val="1B9E77"/>
+                      </a:solidFill>
+                      <a:prstDash val="dash"/>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pn slope exc'!$B$14:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pn slope exc'!$D$14:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.491919596031121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-E698-4A5F-BDE5-6E8233C84A0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="755857903"/>
+        <c:axId val="755857071"/>
+        <c:extLst/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="755857903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="F2F2F2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE" sz="900" b="0"/>
+                  <a:t>secs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="755857071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+        <c:minorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="755857071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="F2F2F2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE" sz="900" b="0" i="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>slope (ST/sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="755857903"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="25000"/>
+              <a:lumOff val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1878119962321656"/>
+          <c:y val="7.7452287031350972E-2"/>
+          <c:w val="0.39058580276308075"/>
+          <c:h val="0.28341185185185186"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="25000"/>
+              <a:lumOff val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -35516,7 +36370,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -53048,15 +53902,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>370149</xdr:colOff>
+      <xdr:colOff>360624</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>409657</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>21570</xdr:rowOff>
+      <xdr:colOff>44974</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9939</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -53268,6 +54122,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>130098</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>283495</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19465</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AED6DF6-D0B2-4793-BC31-6094B5C6F27F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -54175,10 +55067,10 @@
             <v>184.03</v>
           </cell>
           <cell r="C5">
-            <v>151.506949680486</v>
+            <v>151.50683841721499</v>
           </cell>
           <cell r="D5">
-            <v>216.54399928761001</v>
+            <v>216.54403127159</v>
           </cell>
           <cell r="E5">
             <v>15.51</v>
@@ -54192,10 +55084,10 @@
             <v>146.68</v>
           </cell>
           <cell r="C6">
-            <v>90.808399579699397</v>
+            <v>90.808469462109997</v>
           </cell>
           <cell r="D6">
-            <v>202.55092072075499</v>
+            <v>202.55082204353101</v>
           </cell>
           <cell r="E6">
             <v>23.92</v>
@@ -54209,10 +55101,10 @@
             <v>184.81</v>
           </cell>
           <cell r="C7">
-            <v>128.28338969342599</v>
+            <v>128.28353729013401</v>
           </cell>
           <cell r="D7">
-            <v>241.34456183907</v>
+            <v>241.344429878315</v>
           </cell>
           <cell r="E7">
             <v>24.92</v>
@@ -54226,10 +55118,10 @@
             <v>196.31</v>
           </cell>
           <cell r="C8">
-            <v>139.783401363927</v>
+            <v>139.783390452486</v>
           </cell>
           <cell r="D8">
-            <v>252.84052976831401</v>
+            <v>252.840571781113</v>
           </cell>
           <cell r="E8">
             <v>24.93</v>
@@ -54243,10 +55135,10 @@
             <v>184.03</v>
           </cell>
           <cell r="C9">
-            <v>151.50699150927201</v>
+            <v>151.506897643895</v>
           </cell>
           <cell r="D9">
-            <v>216.543988074411</v>
+            <v>216.54397852610199</v>
           </cell>
           <cell r="E9">
             <v>15.51</v>
@@ -54260,10 +55152,10 @@
             <v>223.65</v>
           </cell>
           <cell r="C10">
-            <v>189.32100990096399</v>
+            <v>189.32076094309201</v>
           </cell>
           <cell r="D10">
-            <v>257.98451528172501</v>
+            <v>257.98440541662802</v>
           </cell>
           <cell r="E10">
             <v>16.38</v>
@@ -54277,10 +55169,10 @@
             <v>250.64</v>
           </cell>
           <cell r="C11">
-            <v>206.74646438307099</v>
+            <v>206.74593969084901</v>
           </cell>
           <cell r="D11">
-            <v>294.53480036163103</v>
+            <v>294.53470861677101</v>
           </cell>
           <cell r="E11">
             <v>20.29</v>
@@ -54294,10 +55186,10 @@
             <v>251.81</v>
           </cell>
           <cell r="C12">
-            <v>211.81376536255701</v>
+            <v>211.81135308696099</v>
           </cell>
           <cell r="D12">
-            <v>291.80850172416001</v>
+            <v>291.81011699200002</v>
           </cell>
           <cell r="E12">
             <v>18.86</v>
@@ -54483,70 +55375,70 @@
         </row>
         <row r="2">
           <cell r="A2" t="str">
-            <v>ana_syls0</v>
+            <v>foot_syls1</v>
           </cell>
           <cell r="B2">
-            <v>2.25</v>
+            <v>2.3199999999999998</v>
           </cell>
           <cell r="C2">
-            <v>1.2193754869086899</v>
+            <v>1.40954224352258</v>
           </cell>
           <cell r="D2">
-            <v>3.2871948464253302</v>
+            <v>3.2305699380072102</v>
           </cell>
           <cell r="E2">
-            <v>0.48</v>
+            <v>0.43</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
-            <v>ana_syls1</v>
+            <v>foot_syls2</v>
           </cell>
           <cell r="B3">
-            <v>2.19</v>
+            <v>2.91</v>
           </cell>
           <cell r="C3">
-            <v>3.71627578716653E-2</v>
+            <v>2.0317947390718598</v>
           </cell>
           <cell r="D3">
-            <v>4.3492149985115196</v>
+            <v>3.78116697322687</v>
           </cell>
           <cell r="E3">
-            <v>0.84</v>
+            <v>0.41</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4" t="str">
-            <v>ana_syls2</v>
+            <v>foot_syls3</v>
           </cell>
           <cell r="B4">
-            <v>3.25</v>
+            <v>3.2</v>
           </cell>
           <cell r="C4">
-            <v>1.10274649319997</v>
+            <v>2.33358406032526</v>
           </cell>
           <cell r="D4">
-            <v>5.3896313290389104</v>
+            <v>4.0713630735969897</v>
           </cell>
           <cell r="E4">
-            <v>0.86</v>
+            <v>0.4</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5" t="str">
-            <v>ana_syls3</v>
+            <v>foot_syls4</v>
           </cell>
           <cell r="B5">
-            <v>2.74</v>
+            <v>2.93</v>
           </cell>
           <cell r="C5">
-            <v>0.59682035643766795</v>
+            <v>2.0329467627845199</v>
           </cell>
           <cell r="D5">
-            <v>4.8835889161651904</v>
+            <v>3.8351403664950801</v>
           </cell>
           <cell r="E5">
-            <v>0.86</v>
+            <v>0.42</v>
           </cell>
         </row>
       </sheetData>
@@ -54584,70 +55476,70 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="A2" t="str">
-            <v>ana_syls0</v>
+            <v>foot_syls1</v>
           </cell>
           <cell r="B2">
-            <v>2.67</v>
+            <v>2.97</v>
           </cell>
           <cell r="C2">
-            <v>2.2444539271720498</v>
+            <v>2.0401095455592699</v>
           </cell>
           <cell r="D2">
-            <v>3.09445969557542</v>
+            <v>3.9037741296025401</v>
           </cell>
           <cell r="E2">
-            <v>0.19</v>
+            <v>0.2</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
-            <v>ana_syls1</v>
+            <v>foot_syls2</v>
           </cell>
           <cell r="B3">
-            <v>2.73</v>
+            <v>2.83</v>
           </cell>
           <cell r="C3">
-            <v>1.79172008297501</v>
+            <v>1.9615363862242201</v>
           </cell>
           <cell r="D3">
-            <v>3.662384469864</v>
+            <v>3.68952450221507</v>
           </cell>
           <cell r="E3">
-            <v>0.32</v>
+            <v>0.21</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4" t="str">
-            <v>ana_syls2</v>
+            <v>foot_syls3</v>
           </cell>
           <cell r="B4">
             <v>2.9</v>
           </cell>
           <cell r="C4">
-            <v>1.9889242999987899</v>
+            <v>1.94303337950157</v>
           </cell>
           <cell r="D4">
-            <v>3.8174185660920301</v>
+            <v>3.8523216127305</v>
           </cell>
           <cell r="E4">
-            <v>0.33</v>
+            <v>0.19</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5" t="str">
-            <v>ana_syls3</v>
+            <v>foot_syls4</v>
           </cell>
           <cell r="B5">
-            <v>2.77</v>
+            <v>2.87</v>
           </cell>
           <cell r="C5">
-            <v>1.8541376361439801</v>
+            <v>2.5491215927225501</v>
           </cell>
           <cell r="D5">
-            <v>3.6785445274248301</v>
+            <v>3.18753310101377</v>
           </cell>
           <cell r="E5">
-            <v>0.33</v>
+            <v>0.14000000000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -58679,7 +59571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC0849F-EF38-4D7B-B676-64AFB5DCFB0A}">
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -58979,11 +59871,11 @@
       </c>
       <c r="C16" s="3">
         <f>[17]pn_h_t_b0!C9</f>
-        <v>151.50699150927201</v>
+        <v>151.506897643895</v>
       </c>
       <c r="D16" s="3">
         <f>[17]pn_h_t_b0!D9</f>
-        <v>216.543988074411</v>
+        <v>216.54397852610199</v>
       </c>
       <c r="E16">
         <f>[17]pn_h_t_b0!E9</f>
@@ -58991,7 +59883,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>32.523008490727989</v>
+        <v>32.523102356104999</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.3">
@@ -59005,11 +59897,11 @@
       </c>
       <c r="C17" s="3">
         <f>[17]pn_h_t_b0!C10</f>
-        <v>189.32100990096399</v>
+        <v>189.32076094309201</v>
       </c>
       <c r="D17" s="3">
         <f>[17]pn_h_t_b0!D10</f>
-        <v>257.98451528172501</v>
+        <v>257.98440541662802</v>
       </c>
       <c r="E17">
         <f>[17]pn_h_t_b0!E10</f>
@@ -59017,7 +59909,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>34.32899009903602</v>
+        <v>34.329239056907994</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.3">
@@ -59031,11 +59923,11 @@
       </c>
       <c r="C18" s="3">
         <f>[17]pn_h_t_b0!C11</f>
-        <v>206.74646438307099</v>
+        <v>206.74593969084901</v>
       </c>
       <c r="D18" s="3">
         <f>[17]pn_h_t_b0!D11</f>
-        <v>294.53480036163103</v>
+        <v>294.53470861677101</v>
       </c>
       <c r="E18">
         <f>[17]pn_h_t_b0!E11</f>
@@ -59043,7 +59935,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>43.893535616929</v>
+        <v>43.894060309150973</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.3">
@@ -59057,11 +59949,11 @@
       </c>
       <c r="C19" s="3">
         <f>[17]pn_h_t_b0!C12</f>
-        <v>211.81376536255701</v>
+        <v>211.81135308696099</v>
       </c>
       <c r="D19" s="3">
         <f>[17]pn_h_t_b0!D12</f>
-        <v>291.80850172416001</v>
+        <v>291.81011699200002</v>
       </c>
       <c r="E19">
         <f>[17]pn_h_t_b0!E12</f>
@@ -59069,7 +59961,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>39.996234637442996</v>
+        <v>39.998646913039011</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.3">
@@ -59612,11 +60504,11 @@
       </c>
       <c r="C16" s="3">
         <f>[17]pn_h_t_b0!C5</f>
-        <v>151.506949680486</v>
+        <v>151.50683841721499</v>
       </c>
       <c r="D16" s="3">
         <f>[17]pn_h_t_b0!D5</f>
-        <v>216.54399928761001</v>
+        <v>216.54403127159</v>
       </c>
       <c r="E16" s="3">
         <f>[17]pn_h_t_b0!E5</f>
@@ -59624,7 +60516,7 @@
       </c>
       <c r="F16" s="3">
         <f>B16-C16</f>
-        <v>32.523050319513999</v>
+        <v>32.523161582785008</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.3">
@@ -59638,11 +60530,11 @@
       </c>
       <c r="C17" s="3">
         <f>[17]pn_h_t_b0!C6</f>
-        <v>90.808399579699397</v>
+        <v>90.808469462109997</v>
       </c>
       <c r="D17" s="3">
         <f>[17]pn_h_t_b0!D6</f>
-        <v>202.55092072075499</v>
+        <v>202.55082204353101</v>
       </c>
       <c r="E17" s="3">
         <f>[17]pn_h_t_b0!E6</f>
@@ -59650,7 +60542,7 @@
       </c>
       <c r="F17" s="3">
         <f>B17-C17</f>
-        <v>55.871600420300609</v>
+        <v>55.87153053789001</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.3">
@@ -59664,11 +60556,11 @@
       </c>
       <c r="C18" s="3">
         <f>[17]pn_h_t_b0!C7</f>
-        <v>128.28338969342599</v>
+        <v>128.28353729013401</v>
       </c>
       <c r="D18" s="3">
         <f>[17]pn_h_t_b0!D7</f>
-        <v>241.34456183907</v>
+        <v>241.344429878315</v>
       </c>
       <c r="E18" s="3">
         <f>[17]pn_h_t_b0!E7</f>
@@ -59676,7 +60568,7 @@
       </c>
       <c r="F18" s="3">
         <f>B18-C18</f>
-        <v>56.526610306574014</v>
+        <v>56.526462709865996</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.3">
@@ -59690,11 +60582,11 @@
       </c>
       <c r="C19" s="3">
         <f>[17]pn_h_t_b0!C8</f>
-        <v>139.783401363927</v>
+        <v>139.783390452486</v>
       </c>
       <c r="D19" s="3">
         <f>[17]pn_h_t_b0!D8</f>
-        <v>252.84052976831401</v>
+        <v>252.840571781113</v>
       </c>
       <c r="E19" s="3">
         <f>[17]pn_h_t_b0!E8</f>
@@ -59702,7 +60594,7 @@
       </c>
       <c r="F19" s="3">
         <f>B19-C19</f>
-        <v>56.526598636073004</v>
+        <v>56.526609547513999</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.3">
@@ -59781,7 +60673,7 @@
         <v>0.7</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F9:F25" si="0">B23-C23</f>
+        <f t="shared" ref="F23:F25" si="0">B23-C23</f>
         <v>1.7759811698808627</v>
       </c>
     </row>
@@ -59927,8 +60819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF1DDAF-16D8-40D4-8656-D048765803AC}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59963,28 +60855,28 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="str">
-        <f>RIGHT([19]pn_f0_exc_b0!A2,5)</f>
-        <v>syls0</v>
+        <f>([19]pn_f0_exc_b0!A2)</f>
+        <v>foot_syls1</v>
       </c>
       <c r="B2" s="1">
         <f>[19]pn_f0_exc_b0!B2</f>
-        <v>2.25</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="C2" s="1">
         <f>[19]pn_f0_exc_b0!C2</f>
-        <v>1.2193754869086899</v>
+        <v>1.40954224352258</v>
       </c>
       <c r="D2" s="1">
         <f>[19]pn_f0_exc_b0!D2</f>
-        <v>3.2871948464253302</v>
+        <v>3.2305699380072102</v>
       </c>
       <c r="E2" s="1">
         <f>[19]pn_f0_exc_b0!E2</f>
-        <v>0.48</v>
+        <v>0.43</v>
       </c>
       <c r="F2" s="13">
         <f>B2-C2</f>
-        <v>1.0306245130913101</v>
+        <v>0.91045775647741989</v>
       </c>
       <c r="R2" s="42" t="s">
         <v>24</v>
@@ -59993,28 +60885,28 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str">
-        <f>RIGHT([19]pn_f0_exc_b0!A3,5)</f>
-        <v>syls1</v>
+        <f>([19]pn_f0_exc_b0!A3)</f>
+        <v>foot_syls2</v>
       </c>
       <c r="B3" s="1">
         <f>[19]pn_f0_exc_b0!B3</f>
-        <v>2.19</v>
+        <v>2.91</v>
       </c>
       <c r="C3" s="1">
         <f>[19]pn_f0_exc_b0!C3</f>
-        <v>3.71627578716653E-2</v>
+        <v>2.0317947390718598</v>
       </c>
       <c r="D3" s="1">
         <f>[19]pn_f0_exc_b0!D3</f>
-        <v>4.3492149985115196</v>
+        <v>3.78116697322687</v>
       </c>
       <c r="E3" s="1">
         <f>[19]pn_f0_exc_b0!E3</f>
-        <v>0.84</v>
+        <v>0.41</v>
       </c>
       <c r="F3" s="13">
         <f t="shared" ref="F3:F5" si="0">B3-C3</f>
-        <v>2.1528372421283346</v>
+        <v>0.87820526092814033</v>
       </c>
       <c r="R3" s="44" t="s">
         <v>25</v>
@@ -60023,54 +60915,54 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
-        <f>RIGHT([19]pn_f0_exc_b0!A4,5)</f>
-        <v>syls2</v>
+        <f>([19]pn_f0_exc_b0!A4)</f>
+        <v>foot_syls3</v>
       </c>
       <c r="B4" s="1">
         <f>[19]pn_f0_exc_b0!B4</f>
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="C4" s="1">
         <f>[19]pn_f0_exc_b0!C4</f>
-        <v>1.10274649319997</v>
+        <v>2.33358406032526</v>
       </c>
       <c r="D4" s="1">
         <f>[19]pn_f0_exc_b0!D4</f>
-        <v>5.3896313290389104</v>
+        <v>4.0713630735969897</v>
       </c>
       <c r="E4" s="1">
         <f>[19]pn_f0_exc_b0!E4</f>
-        <v>0.86</v>
+        <v>0.4</v>
       </c>
       <c r="F4" s="13">
         <f t="shared" si="0"/>
-        <v>2.14725350680003</v>
+        <v>0.86641593967474018</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
-        <f>RIGHT([19]pn_f0_exc_b0!A5,5)</f>
-        <v>syls3</v>
+        <f>([19]pn_f0_exc_b0!A5)</f>
+        <v>foot_syls4</v>
       </c>
       <c r="B5" s="1">
         <f>[19]pn_f0_exc_b0!B5</f>
-        <v>2.74</v>
+        <v>2.93</v>
       </c>
       <c r="C5" s="1">
         <f>[19]pn_f0_exc_b0!C5</f>
-        <v>0.59682035643766795</v>
+        <v>2.0329467627845199</v>
       </c>
       <c r="D5" s="1">
         <f>[19]pn_f0_exc_b0!D5</f>
-        <v>4.8835889161651904</v>
+        <v>3.8351403664950801</v>
       </c>
       <c r="E5" s="1">
         <f>[19]pn_f0_exc_b0!E5</f>
-        <v>0.86</v>
+        <v>0.42</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="0"/>
-        <v>2.1431796435623323</v>
+        <v>0.89705323721548025</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -60106,60 +60998,60 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
-        <f>RIGHT([20]pn_lh_slope_b0!A2,5)</f>
-        <v>syls0</v>
+        <f>([20]pn_lh_slope_b0!A2)</f>
+        <v>foot_syls1</v>
       </c>
       <c r="B8" s="1">
         <f>[20]pn_lh_slope_b0!B2</f>
-        <v>2.67</v>
+        <v>2.97</v>
       </c>
       <c r="C8" s="1">
         <f>[20]pn_lh_slope_b0!C2</f>
-        <v>2.2444539271720498</v>
+        <v>2.0401095455592699</v>
       </c>
       <c r="D8" s="1">
         <f>[20]pn_lh_slope_b0!D2</f>
-        <v>3.09445969557542</v>
+        <v>3.9037741296025401</v>
       </c>
       <c r="E8" s="1">
         <f>[20]pn_lh_slope_b0!E2</f>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="F8" s="13">
         <f>B8-C8</f>
-        <v>0.42554607282795009</v>
+        <v>0.92989045444073026</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
-        <f>RIGHT([20]pn_lh_slope_b0!A3,5)</f>
-        <v>syls1</v>
+        <f>([20]pn_lh_slope_b0!A3)</f>
+        <v>foot_syls2</v>
       </c>
       <c r="B9" s="1">
         <f>[20]pn_lh_slope_b0!B3</f>
-        <v>2.73</v>
+        <v>2.83</v>
       </c>
       <c r="C9" s="1">
         <f>[20]pn_lh_slope_b0!C3</f>
-        <v>1.79172008297501</v>
+        <v>1.9615363862242201</v>
       </c>
       <c r="D9" s="1">
         <f>[20]pn_lh_slope_b0!D3</f>
-        <v>3.662384469864</v>
+        <v>3.68952450221507</v>
       </c>
       <c r="E9" s="1">
         <f>[20]pn_lh_slope_b0!E3</f>
-        <v>0.32</v>
+        <v>0.21</v>
       </c>
       <c r="F9" s="13">
         <f>B9-C9</f>
-        <v>0.93827991702499003</v>
+        <v>0.86846361377577996</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
-        <f>RIGHT([20]pn_lh_slope_b0!A4,5)</f>
-        <v>syls2</v>
+        <f>([20]pn_lh_slope_b0!A4)</f>
+        <v>foot_syls3</v>
       </c>
       <c r="B10" s="1">
         <f>[20]pn_lh_slope_b0!B4</f>
@@ -60167,45 +61059,45 @@
       </c>
       <c r="C10" s="1">
         <f>[20]pn_lh_slope_b0!C4</f>
-        <v>1.9889242999987899</v>
+        <v>1.94303337950157</v>
       </c>
       <c r="D10" s="1">
         <f>[20]pn_lh_slope_b0!D4</f>
-        <v>3.8174185660920301</v>
+        <v>3.8523216127305</v>
       </c>
       <c r="E10" s="1">
         <f>[20]pn_lh_slope_b0!E4</f>
-        <v>0.33</v>
+        <v>0.19</v>
       </c>
       <c r="F10" s="13">
         <f>B10-C10</f>
-        <v>0.91107570000120996</v>
+        <v>0.95696662049842995</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
-        <f>RIGHT([20]pn_lh_slope_b0!A5,5)</f>
-        <v>syls3</v>
+        <f>([20]pn_lh_slope_b0!A5)</f>
+        <v>foot_syls4</v>
       </c>
       <c r="B11" s="1">
         <f>[20]pn_lh_slope_b0!B5</f>
-        <v>2.77</v>
+        <v>2.87</v>
       </c>
       <c r="C11" s="1">
         <f>[20]pn_lh_slope_b0!C5</f>
-        <v>1.8541376361439801</v>
+        <v>2.5491215927225501</v>
       </c>
       <c r="D11" s="1">
         <f>[20]pn_lh_slope_b0!D5</f>
-        <v>3.6785445274248301</v>
+        <v>3.18753310101377</v>
       </c>
       <c r="E11" s="1">
         <f>[20]pn_lh_slope_b0!E5</f>
-        <v>0.33</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F11" s="13">
         <f>B11-C11</f>
-        <v>0.91586236385601993</v>
+        <v>0.32087840727744998</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -60219,7 +61111,7 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f>A15</f>
-        <v>syls0</v>
+        <v>foot_syls1</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -60235,24 +61127,24 @@
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f>A8</f>
-        <v>syls0</v>
+        <v>foot_syls1</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="1">
         <f>B8</f>
-        <v>2.67</v>
+        <v>2.97</v>
       </c>
       <c r="D15" s="2">
         <f>EXP(C15)</f>
-        <v>14.439969192802881</v>
+        <v>19.491919596031121</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f>A17</f>
-        <v>syls1</v>
+        <v>foot_syls2</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -60270,7 +61162,7 @@
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
         <f>A9</f>
-        <v>syls1</v>
+        <v>foot_syls2</v>
       </c>
       <c r="B17">
         <f>B15</f>
@@ -60278,11 +61170,11 @@
       </c>
       <c r="C17" s="1">
         <f>B9</f>
-        <v>2.73</v>
+        <v>2.83</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" ref="D17" si="3">EXP(C17)</f>
-        <v>15.332887019907195</v>
+        <v>16.945460824541019</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="13"/>
@@ -60290,7 +61182,7 @@
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f>A19</f>
-        <v>syls2</v>
+        <v>foot_syls3</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -60308,7 +61200,7 @@
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="str">
         <f>A10</f>
-        <v>syls2</v>
+        <v>foot_syls3</v>
       </c>
       <c r="B19">
         <f>B17</f>
@@ -60331,7 +61223,7 @@
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="str">
         <f>A21</f>
-        <v>syls3</v>
+        <v>foot_syls4</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -60347,7 +61239,7 @@
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="str">
         <f>A11</f>
-        <v>syls3</v>
+        <v>foot_syls4</v>
       </c>
       <c r="B21">
         <f>B19</f>
@@ -60355,11 +61247,11 @@
       </c>
       <c r="C21" s="1">
         <f>B11</f>
-        <v>2.77</v>
+        <v>2.87</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" ref="D21" si="7">EXP(C21)</f>
-        <v>15.958634009794029</v>
+        <v>17.637018199837321</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
@@ -60378,11 +61270,11 @@
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>A8</f>
-        <v>syls0</v>
+        <v>foot_syls1</v>
       </c>
       <c r="B24" s="1">
         <f>EXP(B8)</f>
-        <v>14.439969192802881</v>
+        <v>19.491919596031121</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -60392,11 +61284,11 @@
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>A9</f>
-        <v>syls1</v>
+        <v>foot_syls2</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" ref="B25:B27" si="8">EXP(B9)</f>
-        <v>15.332887019907195</v>
+        <v>16.945460824541019</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -60406,7 +61298,7 @@
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>A10</f>
-        <v>syls2</v>
+        <v>foot_syls3</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="8"/>
@@ -60420,11 +61312,11 @@
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>A11</f>
-        <v>syls3</v>
+        <v>foot_syls4</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="8"/>
-        <v>15.958634009794029</v>
+        <v>17.637018199837321</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>

</xml_diff>